<commit_message>
cambio de plantilla, y fetrch pacientes cuando es pasante
</commit_message>
<xml_diff>
--- a/public/plantilla.xlsx
+++ b/public/plantilla.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28005"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carlos\Documents\Github\ssss\UDIPSAI-Frontend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23949B7C-AC1D-4DEE-A654-A826C4619ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB539C1D-989B-46E3-B0F4-C48B399DA056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F25F2A54-0E5A-43B4-BC39-1DD5D9987810}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB57AABC-52A1-407C-909B-68D3503BCDA1}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PSICOLOGÍA_EDUCATIVA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PSICOLOGÍA_EDUCATIVA!$A$1:$T$1</definedName>
+    <definedName name="_Hlk65870024" localSheetId="0">PSICOLOGÍA_EDUCATIVA!#REF!</definedName>
+    <definedName name="_Hlk77071873" localSheetId="0">PSICOLOGÍA_EDUCATIVA!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PSICOLOGÍA_EDUCATIVA!#REF!</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +33,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,105 +42,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Cedula</t>
-  </si>
-  <si>
-    <t>NombresApellidos</t>
-  </si>
-  <si>
-    <t>Edad</t>
-  </si>
-  <si>
-    <t>Domicilio</t>
-  </si>
-  <si>
-    <t>Cuidad</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>InstitucionEducativa</t>
-  </si>
-  <si>
-    <t>TipoInstitucion</t>
-  </si>
-  <si>
-    <t>Proyecto</t>
-  </si>
-  <si>
-    <t>Jornada</t>
-  </si>
-  <si>
-    <t>DireccionInstitucion</t>
-  </si>
-  <si>
-    <t>AnioEducacion</t>
-  </si>
-  <si>
-    <t>Paralelo</t>
-  </si>
-  <si>
-    <t>PerteneceInclusion</t>
-  </si>
-  <si>
-    <t>TieneDiscapacidad</t>
-  </si>
-  <si>
-    <t>PortadorCarnet</t>
-  </si>
-  <si>
-    <t>Diagnostico</t>
-  </si>
-  <si>
-    <t>MotivoConsulta</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>FechaApertura</t>
-  </si>
-  <si>
-    <t>FechaNacimiento</t>
-  </si>
-  <si>
-    <t>PacienteEstado</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>CÓDIGO</t>
+  </si>
+  <si>
+    <t>FECHA DE APERTURA DE LA FICHA</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS</t>
+  </si>
+  <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t>FECHA DE NACIMIENTO</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>CÉDULA</t>
+  </si>
+  <si>
+    <t>DOMICILIO</t>
+  </si>
+  <si>
+    <t>TELÉFONO</t>
+  </si>
+  <si>
+    <t>CELULAR</t>
+  </si>
+  <si>
+    <t>INSTITUCIÓN EDUCATIVA</t>
+  </si>
+  <si>
+    <t>TIPO DE INSTITUCIÓN</t>
+  </si>
+  <si>
+    <t>JORNADA</t>
+  </si>
+  <si>
+    <t>AÑO EGB</t>
+  </si>
+  <si>
+    <t>PARALELO</t>
+  </si>
+  <si>
+    <t>PERTENECE A INCLUSIÓN</t>
+  </si>
+  <si>
+    <t>TIENE DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>PORTADOR DE CARNÉ</t>
+  </si>
+  <si>
+    <t>DIAGNÓSTICO</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>SEDE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-C0A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+  </numFmts>
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFED7D31"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,17 +170,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -166,7 +252,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -461,93 +547,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199BBFC8-1365-401B-891A-77BA87124480}">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="45" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="16" style="10" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="11" customWidth="1"/>
+    <col min="19" max="19" width="53.5703125" style="10" customWidth="1"/>
+    <col min="20" max="20" width="53.42578125" style="10" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" style="5" customWidth="1"/>
+    <col min="22" max="23" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.7109375" style="5" customWidth="1"/>
+    <col min="25" max="26" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="116" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="117" max="1016" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1017" max="1027" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1116" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1117" max="1127" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1128" max="1128" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1129" max="1216" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1217" max="1227" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1228" max="1228" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1229" max="1327" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1328" max="1328" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1329" max="1427" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1428" max="1428" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1429" max="1527" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1528" max="1528" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1529" max="1627" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1628" max="1628" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1629" max="1727" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1728" max="1728" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1729" max="1827" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1828" max="1828" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1829" max="1927" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1928" max="1928" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1929" max="2027" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2028" max="2028" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2029" max="2126" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2127" max="2136" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2137" max="2227" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2228" max="2228" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2229" max="2327" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2427" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2428" max="2428" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2429" max="2527" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2528" max="2528" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2529" max="2627" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2628" max="2628" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2629" max="2727" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2728" max="2728" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2729" max="2827" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2828" max="2828" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2829" max="2927" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2928" max="2928" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2929" max="3027" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3028" max="3028" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3029" max="3043" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3044" max="10016" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10017" max="16376" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16377" max="16384" width="16.28515625" style="5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <autoFilter ref="A1:T1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="0" scale="65" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>